<commit_message>
getting the last version
</commit_message>
<xml_diff>
--- a/src/excelExportAndFileIO/jeu_de_test_BR.xlsx
+++ b/src/excelExportAndFileIO/jeu_de_test_BR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galinabikono\workspace\seleniumtest\src\excelExportAndFileIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galinabikono\workspace\gitlab\src\excelExportAndFileIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Nome</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Modelo</t>
   </si>
   <si>
-    <t>Kwid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validade do contrato </t>
   </si>
   <si>
@@ -239,6 +236,15 @@
   </si>
   <si>
     <t>Código de segurança</t>
+  </si>
+  <si>
+    <t>KWID 1.0</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>Razão Social</t>
   </si>
 </sst>
 </file>
@@ -617,20 +623,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="23" max="23" width="24.140625" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
     <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,70 +660,76 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
       <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
       <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
       <c r="T1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
-        <v>38</v>
-      </c>
       <c r="Y1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
-        <v>43</v>
+      <c r="AC1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -736,19 +749,19 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="K2" s="1">
-        <v>43101</v>
+        <v>43187</v>
       </c>
       <c r="L2" s="5">
         <v>6132223990</v>
@@ -757,13 +770,13 @@
         <v>6232223999</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="1">
         <v>31118</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2">
         <v>3</v>
@@ -772,22 +785,22 @@
         <v>86041230</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="X2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y2" s="3">
         <v>4917610000000000</v>

</xml_diff>